<commit_message>
Added PTVs to outputs
</commit_message>
<xml_diff>
--- a/Data/20250929_BARD1_OddsRatios_supptable.xlsx
+++ b/Data/20250929_BARD1_OddsRatios_supptable.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1775,7 +1775,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>bridges</t>
+          <t>carriers</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1785,66 +1785,66 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>bridges_all</t>
+          <t>carriers_all</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>miss</t>
+          <t>ptv</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F20" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G20" t="n">
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>583</v>
+        <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>60466</v>
+        <v>39553</v>
       </c>
       <c r="J20" t="n">
-        <v>53461</v>
+        <v>35867</v>
       </c>
       <c r="K20" t="n">
-        <v>2.134154617528004</v>
+        <v>0.9974894445427654</v>
       </c>
       <c r="L20" t="n">
-        <v>1.384146802486698</v>
+        <v>0.5443149304576366</v>
       </c>
       <c r="M20" t="n">
-        <v>3.290558431615398</v>
+        <v>1.827958661978455</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0003914898225370895</v>
+        <v>1</v>
       </c>
       <c r="O20" t="n">
-        <v>0.9705932296329269</v>
+        <v>0.4534042929739843</v>
       </c>
       <c r="P20" t="n">
-        <v>0.8670480456036038</v>
+        <v>0.015210666496138</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.086504054978241</v>
+        <v>13.51521663691954</v>
       </c>
       <c r="R20" t="n">
-        <v>0.6043030775318811</v>
+        <v>0.4755704644595006</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>bridges</t>
+          <t>carriers</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1854,124 +1854,124 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>bridges_pop</t>
+          <t>carriers_pop</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>miss</t>
+          <t>ptv</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="F21" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G21" t="n">
-        <v>503</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>549</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>48826</v>
+        <v>32247</v>
       </c>
       <c r="J21" t="n">
-        <v>50703</v>
+        <v>32544</v>
       </c>
       <c r="K21" t="n">
-        <v>1.923041913006276</v>
+        <v>1.06527739014482</v>
       </c>
       <c r="L21" t="n">
-        <v>1.204008410728578</v>
+        <v>0.5589940916495463</v>
       </c>
       <c r="M21" t="n">
-        <v>3.071482031376367</v>
+        <v>2.030103600209815</v>
       </c>
       <c r="N21" t="n">
-        <v>0.005961495485255401</v>
+        <v>0.8708398648035731</v>
       </c>
       <c r="O21" t="n">
-        <v>0.9514328677791708</v>
+        <v>1.009210159084566</v>
       </c>
       <c r="P21" t="n">
-        <v>0.8424886707386938</v>
+        <v>0.02002467099348533</v>
       </c>
       <c r="Q21" t="n">
-        <v>1.074464895886135</v>
+        <v>50.86251582015247</v>
       </c>
       <c r="R21" t="n">
-        <v>0.4383648510118568</v>
+        <v>1</v>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>bridges</t>
+          <t>carriers</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>cc_pop_er_cases</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>bridges_all</t>
+          <t>carriers_cc_pop_er_cases</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ring</t>
+          <t>ptv</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G22" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>89</v>
+        <v>864</v>
       </c>
       <c r="I22" t="n">
-        <v>60466</v>
+        <v>3805</v>
       </c>
       <c r="J22" t="n">
-        <v>53461</v>
+        <v>32544</v>
       </c>
       <c r="K22" t="n">
-        <v>6.189048390831211</v>
+        <v>0.4501556124213293</v>
       </c>
       <c r="L22" t="n">
-        <v>0.7614425140487651</v>
+        <v>0.06024576919494917</v>
       </c>
       <c r="M22" t="n">
-        <v>50.3049400018098</v>
+        <v>3.363556945197255</v>
       </c>
       <c r="N22" t="n">
-        <v>0.07445219212602244</v>
+        <v>0.7154113738522967</v>
       </c>
       <c r="O22" t="n">
-        <v>0.7550042980789278</v>
+        <v>0.004949627682873412</v>
       </c>
       <c r="P22" t="n">
-        <v>0.5557868252581363</v>
+        <v>0.0003092823872473706</v>
       </c>
       <c r="Q22" t="n">
-        <v>1.025629727464126</v>
+        <v>0.07921179869667831</v>
       </c>
       <c r="R22" t="n">
-        <v>0.07299092375667891</v>
+        <v>1.745491773758545e-41</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -1987,64 +1987,64 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ring</t>
+          <t>miss</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="G23" t="n">
-        <v>64</v>
+        <v>640</v>
       </c>
       <c r="H23" t="n">
-        <v>88</v>
+        <v>583</v>
       </c>
       <c r="I23" t="n">
-        <v>48826</v>
+        <v>60466</v>
       </c>
       <c r="J23" t="n">
-        <v>50703</v>
+        <v>53461</v>
       </c>
       <c r="K23" t="n">
-        <v>7.269098431163724</v>
+        <v>2.134154617528004</v>
       </c>
       <c r="L23" t="n">
-        <v>0.8943176831196231</v>
+        <v>1.384146802486698</v>
       </c>
       <c r="M23" t="n">
-        <v>59.08391726933931</v>
+        <v>3.290558431615398</v>
       </c>
       <c r="N23" t="n">
-        <v>0.03576073743865427</v>
+        <v>0.0003914898225370895</v>
       </c>
       <c r="O23" t="n">
-        <v>0.7552310058351921</v>
+        <v>0.9705932296329269</v>
       </c>
       <c r="P23" t="n">
-        <v>0.5471903711436676</v>
+        <v>0.8670480456036038</v>
       </c>
       <c r="Q23" t="n">
-        <v>1.042368254731372</v>
+        <v>1.086504054978241</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0887246736350078</v>
+        <v>0.6043030775318811</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -2056,60 +2056,60 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>ard</t>
+          <t>miss</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="F24" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="G24" t="n">
-        <v>114</v>
+        <v>503</v>
       </c>
       <c r="H24" t="n">
-        <v>104</v>
+        <v>549</v>
       </c>
       <c r="I24" t="n">
-        <v>60466</v>
+        <v>48826</v>
       </c>
       <c r="J24" t="n">
-        <v>53461</v>
+        <v>50703</v>
       </c>
       <c r="K24" t="n">
-        <v>7.073198160949955</v>
+        <v>1.923041913006276</v>
       </c>
       <c r="L24" t="n">
-        <v>1.62627755717022</v>
+        <v>1.204008410728578</v>
       </c>
       <c r="M24" t="n">
-        <v>30.76358768125655</v>
+        <v>3.071482031376367</v>
       </c>
       <c r="N24" t="n">
-        <v>0.001789206064041027</v>
+        <v>0.005961495485255401</v>
       </c>
       <c r="O24" t="n">
-        <v>0.9691641710917006</v>
+        <v>0.9514328677791708</v>
       </c>
       <c r="P24" t="n">
-        <v>0.7427864969640958</v>
+        <v>0.8424886707386938</v>
       </c>
       <c r="Q24" t="n">
-        <v>1.264534552481593</v>
+        <v>1.074464895886135</v>
       </c>
       <c r="R24" t="n">
-        <v>0.8387021143086167</v>
+        <v>0.4383648510118568</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2125,64 +2125,64 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>ard</t>
+          <t>ring</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="H25" t="n">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="I25" t="n">
-        <v>48826</v>
+        <v>60466</v>
       </c>
       <c r="J25" t="n">
-        <v>50703</v>
+        <v>53461</v>
       </c>
       <c r="K25" t="n">
-        <v>6.74987711465203</v>
+        <v>6.189048390831211</v>
       </c>
       <c r="L25" t="n">
-        <v>1.523138358105092</v>
+        <v>0.7614425140487651</v>
       </c>
       <c r="M25" t="n">
-        <v>29.91247697260063</v>
+        <v>50.3049400018098</v>
       </c>
       <c r="N25" t="n">
-        <v>0.003601775021850573</v>
+        <v>0.07445219212602244</v>
       </c>
       <c r="O25" t="n">
-        <v>0.9849146622489877</v>
+        <v>0.7550042980789278</v>
       </c>
       <c r="P25" t="n">
-        <v>0.7402972297852755</v>
+        <v>0.5557868252581363</v>
       </c>
       <c r="Q25" t="n">
-        <v>1.310361369573687</v>
+        <v>1.025629727464126</v>
       </c>
       <c r="R25" t="n">
-        <v>0.942026303990013</v>
+        <v>0.07299092375667891</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -2194,60 +2194,60 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>brct</t>
+          <t>ring</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F26" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>174</v>
+        <v>64</v>
       </c>
       <c r="H26" t="n">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="I26" t="n">
-        <v>60466</v>
+        <v>48826</v>
       </c>
       <c r="J26" t="n">
-        <v>53461</v>
+        <v>50703</v>
       </c>
       <c r="K26" t="n">
-        <v>1.675231143382884</v>
+        <v>7.269098431163724</v>
       </c>
       <c r="L26" t="n">
-        <v>0.9608387516784721</v>
+        <v>0.8943176831196231</v>
       </c>
       <c r="M26" t="n">
-        <v>2.920780806204448</v>
+        <v>59.08391726933931</v>
       </c>
       <c r="N26" t="n">
-        <v>0.07842322022575923</v>
+        <v>0.03576073743865427</v>
       </c>
       <c r="O26" t="n">
-        <v>1.148075074631802</v>
+        <v>0.7552310058351921</v>
       </c>
       <c r="P26" t="n">
-        <v>0.916237183045236</v>
+        <v>0.5471903711436676</v>
       </c>
       <c r="Q26" t="n">
-        <v>1.438575514486343</v>
+        <v>1.042368254731372</v>
       </c>
       <c r="R26" t="n">
-        <v>0.2528646886659039</v>
+        <v>0.0887246736350078</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
@@ -2263,64 +2263,64 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>brct</t>
+          <t>ard</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F27" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="H27" t="n">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="I27" t="n">
-        <v>48826</v>
+        <v>60466</v>
       </c>
       <c r="J27" t="n">
-        <v>50703</v>
+        <v>53461</v>
       </c>
       <c r="K27" t="n">
-        <v>1.20240725929024</v>
+        <v>7.073198160949955</v>
       </c>
       <c r="L27" t="n">
-        <v>0.6507462379832341</v>
+        <v>1.62627755717022</v>
       </c>
       <c r="M27" t="n">
-        <v>2.221731195365159</v>
+        <v>30.76358768125655</v>
       </c>
       <c r="N27" t="n">
-        <v>0.6400163153212011</v>
+        <v>0.001789206064041027</v>
       </c>
       <c r="O27" t="n">
-        <v>1.054542518806697</v>
+        <v>0.9691641710917006</v>
       </c>
       <c r="P27" t="n">
-        <v>0.8266935651369767</v>
+        <v>0.7427864969640958</v>
       </c>
       <c r="Q27" t="n">
-        <v>1.345190008569761</v>
+        <v>1.264534552481593</v>
       </c>
       <c r="R27" t="n">
-        <v>0.7094862447453387</v>
+        <v>0.8387021143086167</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -2332,60 +2332,60 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>structured</t>
+          <t>ard</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="F28" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G28" t="n">
-        <v>364</v>
+        <v>92</v>
       </c>
       <c r="H28" t="n">
-        <v>327</v>
+        <v>97</v>
       </c>
       <c r="I28" t="n">
-        <v>60466</v>
+        <v>48826</v>
       </c>
       <c r="J28" t="n">
-        <v>53461</v>
+        <v>50703</v>
       </c>
       <c r="K28" t="n">
-        <v>2.371128928954815</v>
+        <v>6.74987711465203</v>
       </c>
       <c r="L28" t="n">
-        <v>1.452977051467391</v>
+        <v>1.523138358105092</v>
       </c>
       <c r="M28" t="n">
-        <v>3.869470885344248</v>
+        <v>29.91247697260063</v>
       </c>
       <c r="N28" t="n">
-        <v>0.0003252321435773081</v>
+        <v>0.003601775021850573</v>
       </c>
       <c r="O28" t="n">
-        <v>0.984191181416584</v>
+        <v>0.9849146622489877</v>
       </c>
       <c r="P28" t="n">
-        <v>0.8472808609875282</v>
+        <v>0.7402972297852755</v>
       </c>
       <c r="Q28" t="n">
-        <v>1.143224550651603</v>
+        <v>1.310361369573687</v>
       </c>
       <c r="R28" t="n">
-        <v>0.8484539330284671</v>
+        <v>0.942026303990013</v>
       </c>
       <c r="S28" t="inlineStr">
         <is>
@@ -2401,64 +2401,64 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>structured</t>
+          <t>brct</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F29" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G29" t="n">
-        <v>287</v>
+        <v>174</v>
       </c>
       <c r="H29" t="n">
-        <v>314</v>
+        <v>134</v>
       </c>
       <c r="I29" t="n">
-        <v>48826</v>
+        <v>60466</v>
       </c>
       <c r="J29" t="n">
-        <v>50703</v>
+        <v>53461</v>
       </c>
       <c r="K29" t="n">
-        <v>1.982481390317379</v>
+        <v>1.675231143382884</v>
       </c>
       <c r="L29" t="n">
-        <v>1.183380243572501</v>
+        <v>0.9608387516784721</v>
       </c>
       <c r="M29" t="n">
-        <v>3.321191547942169</v>
+        <v>2.920780806204448</v>
       </c>
       <c r="N29" t="n">
-        <v>0.008475939357638365</v>
+        <v>0.07842322022575923</v>
       </c>
       <c r="O29" t="n">
-        <v>0.9491497951519513</v>
+        <v>1.148075074631802</v>
       </c>
       <c r="P29" t="n">
-        <v>0.808375038973789</v>
+        <v>0.916237183045236</v>
       </c>
       <c r="Q29" t="n">
-        <v>1.114439820878987</v>
+        <v>1.438575514486343</v>
       </c>
       <c r="R29" t="n">
-        <v>0.5394371689781419</v>
+        <v>0.2528646886659039</v>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -2470,60 +2470,60 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>idr</t>
+          <t>brct</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F30" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G30" t="n">
-        <v>232</v>
+        <v>131</v>
       </c>
       <c r="H30" t="n">
-        <v>235</v>
+        <v>129</v>
       </c>
       <c r="I30" t="n">
-        <v>60466</v>
+        <v>48826</v>
       </c>
       <c r="J30" t="n">
-        <v>53461</v>
+        <v>50703</v>
       </c>
       <c r="K30" t="n">
-        <v>1.620941245217698</v>
+        <v>1.20240725929024</v>
       </c>
       <c r="L30" t="n">
-        <v>0.5994273809089213</v>
+        <v>0.6507462379832341</v>
       </c>
       <c r="M30" t="n">
-        <v>4.383267438440757</v>
+        <v>2.221731195365159</v>
       </c>
       <c r="N30" t="n">
-        <v>0.4672775844353211</v>
+        <v>0.6400163153212011</v>
       </c>
       <c r="O30" t="n">
-        <v>0.8728627517768029</v>
+        <v>1.054542518806697</v>
       </c>
       <c r="P30" t="n">
-        <v>0.7277875346586922</v>
+        <v>0.8266935651369767</v>
       </c>
       <c r="Q30" t="n">
-        <v>1.046856873959338</v>
+        <v>1.345190008569761</v>
       </c>
       <c r="R30" t="n">
-        <v>0.1498162608137575</v>
+        <v>0.7094862447453387</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
@@ -2539,129 +2539,129 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>idr</t>
+          <t>structured</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G31" t="n">
-        <v>176</v>
+        <v>364</v>
       </c>
       <c r="H31" t="n">
-        <v>214</v>
+        <v>327</v>
       </c>
       <c r="I31" t="n">
-        <v>48826</v>
+        <v>60466</v>
       </c>
       <c r="J31" t="n">
-        <v>50703</v>
+        <v>53461</v>
       </c>
       <c r="K31" t="n">
-        <v>2.076885266046778</v>
+        <v>2.371128928954815</v>
       </c>
       <c r="L31" t="n">
-        <v>0.6253630285533007</v>
+        <v>1.452977051467391</v>
       </c>
       <c r="M31" t="n">
-        <v>6.897517460059699</v>
+        <v>3.869470885344248</v>
       </c>
       <c r="N31" t="n">
-        <v>0.2586730222110951</v>
+        <v>0.0003252321435773081</v>
       </c>
       <c r="O31" t="n">
-        <v>0.8540462776267126</v>
+        <v>0.984191181416584</v>
       </c>
       <c r="P31" t="n">
-        <v>0.6993534894171208</v>
+        <v>0.8472808609875282</v>
       </c>
       <c r="Q31" t="n">
-        <v>1.042956180766271</v>
+        <v>1.143224550651603</v>
       </c>
       <c r="R31" t="n">
-        <v>0.1279244504485124</v>
+        <v>0.8484539330284671</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>carriers+bridges</t>
+          <t>bridges</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>carriers_all+bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>ard</t>
+          <t>structured</t>
         </is>
       </c>
       <c r="E32" t="n">
+        <v>42</v>
+      </c>
+      <c r="F32" t="n">
         <v>22</v>
       </c>
-      <c r="F32" t="n">
-        <v>5</v>
-      </c>
       <c r="G32" t="n">
-        <v>166</v>
+        <v>287</v>
       </c>
       <c r="H32" t="n">
-        <v>159</v>
+        <v>314</v>
       </c>
       <c r="I32" t="n">
-        <v>100019</v>
+        <v>48826</v>
       </c>
       <c r="J32" t="n">
-        <v>89328</v>
+        <v>50703</v>
       </c>
       <c r="K32" t="n">
-        <v>3.929685359781641</v>
+        <v>1.982481390317379</v>
       </c>
       <c r="L32" t="n">
-        <v>1.488077837107677</v>
+        <v>1.183380243572501</v>
       </c>
       <c r="M32" t="n">
-        <v>10.37743231019223</v>
+        <v>3.321191547942169</v>
       </c>
       <c r="N32" t="n">
-        <v>0.003124934066074294</v>
+        <v>0.008475939357638365</v>
       </c>
       <c r="O32" t="n">
-        <v>0.9324296308229738</v>
+        <v>0.9491497951519513</v>
       </c>
       <c r="P32" t="n">
-        <v>0.750033348347161</v>
+        <v>0.808375038973789</v>
       </c>
       <c r="Q32" t="n">
-        <v>1.159181812852201</v>
+        <v>1.114439820878987</v>
       </c>
       <c r="R32" t="n">
-        <v>0.5410616604028184</v>
+        <v>0.5394371689781419</v>
       </c>
       <c r="S32" t="inlineStr">
         <is>
@@ -2672,134 +2672,134 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>carriers+bridges</t>
+          <t>bridges</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>carriers_pop+bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ard</t>
+          <t>idr</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F33" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G33" t="n">
-        <v>133</v>
+        <v>232</v>
       </c>
       <c r="H33" t="n">
-        <v>147</v>
+        <v>235</v>
       </c>
       <c r="I33" t="n">
-        <v>81073</v>
+        <v>60466</v>
       </c>
       <c r="J33" t="n">
-        <v>83247</v>
+        <v>53461</v>
       </c>
       <c r="K33" t="n">
-        <v>3.491172153491298</v>
+        <v>1.620941245217698</v>
       </c>
       <c r="L33" t="n">
-        <v>1.287966744809779</v>
+        <v>0.5994273809089213</v>
       </c>
       <c r="M33" t="n">
-        <v>9.463196976497366</v>
+        <v>4.383267438440757</v>
       </c>
       <c r="N33" t="n">
-        <v>0.009761027862927318</v>
+        <v>0.4672775844353211</v>
       </c>
       <c r="O33" t="n">
-        <v>0.929023402189561</v>
+        <v>0.8728627517768029</v>
       </c>
       <c r="P33" t="n">
-        <v>0.7346401305548933</v>
+        <v>0.7277875346586922</v>
       </c>
       <c r="Q33" t="n">
-        <v>1.174839824178888</v>
+        <v>1.046856873959338</v>
       </c>
       <c r="R33" t="n">
-        <v>0.5501824510822202</v>
+        <v>0.1498162608137575</v>
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>carriers+bridges</t>
+          <t>bridges</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>carriers_all+bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>brct</t>
+          <t>idr</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G34" t="n">
-        <v>576</v>
+        <v>176</v>
       </c>
       <c r="H34" t="n">
-        <v>486</v>
+        <v>214</v>
       </c>
       <c r="I34" t="n">
-        <v>100019</v>
+        <v>48826</v>
       </c>
       <c r="J34" t="n">
-        <v>89328</v>
+        <v>50703</v>
       </c>
       <c r="K34" t="n">
-        <v>1.587751660517835</v>
+        <v>2.076885266046778</v>
       </c>
       <c r="L34" t="n">
-        <v>0.9907813391008043</v>
+        <v>0.6253630285533007</v>
       </c>
       <c r="M34" t="n">
-        <v>2.544411401374462</v>
+        <v>6.897517460059699</v>
       </c>
       <c r="N34" t="n">
-        <v>0.0635612054843895</v>
+        <v>0.2586730222110951</v>
       </c>
       <c r="O34" t="n">
-        <v>1.05850110701189</v>
+        <v>0.8540462776267126</v>
       </c>
       <c r="P34" t="n">
-        <v>0.9378142779619217</v>
+        <v>0.6993534894171208</v>
       </c>
       <c r="Q34" t="n">
-        <v>1.194719060985432</v>
+        <v>1.042956180766271</v>
       </c>
       <c r="R34" t="n">
-        <v>0.3714346897558351</v>
+        <v>0.1279244504485124</v>
       </c>
       <c r="S34" t="inlineStr">
         <is>
@@ -2810,138 +2810,138 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>carriers+bridges</t>
+          <t>bridges</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>carriers_pop+bridges_pop</t>
+          <t>bridges_all</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>brct</t>
+          <t>ptv</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="F35" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G35" t="n">
-        <v>447</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>453</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>81073</v>
+        <v>60466</v>
       </c>
       <c r="J35" t="n">
-        <v>83247</v>
+        <v>53461</v>
       </c>
       <c r="K35" t="n">
-        <v>1.254996525764846</v>
+        <v>2.554210447009706</v>
       </c>
       <c r="L35" t="n">
-        <v>0.7545987738475224</v>
+        <v>1.494249073164481</v>
       </c>
       <c r="M35" t="n">
-        <v>2.087223481229888</v>
+        <v>4.366066624888171</v>
       </c>
       <c r="N35" t="n">
-        <v>0.4388720879615608</v>
+        <v>0.0004275499216491426</v>
       </c>
       <c r="O35" t="n">
-        <v>1.013215136093111</v>
+        <v>0.8841497701187444</v>
       </c>
       <c r="P35" t="n">
-        <v>0.8887884914462424</v>
+        <v>0.01754346004557585</v>
       </c>
       <c r="Q35" t="n">
-        <v>1.155060986824529</v>
+        <v>44.55910145263299</v>
       </c>
       <c r="R35" t="n">
-        <v>0.8672748777633897</v>
+        <v>1</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>carriers+bridges</t>
+          <t>bridges</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>carriers_all+bridges_all</t>
+          <t>bridges_pop</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>idr</t>
+          <t>ptv</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F36" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G36" t="n">
-        <v>558</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>556</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>100019</v>
+        <v>48826</v>
       </c>
       <c r="J36" t="n">
-        <v>89328</v>
+        <v>50703</v>
       </c>
       <c r="K36" t="n">
-        <v>1.442716653066687</v>
+        <v>2.36534155299772</v>
       </c>
       <c r="L36" t="n">
-        <v>0.7223737953440815</v>
+        <v>1.358810112958883</v>
       </c>
       <c r="M36" t="n">
-        <v>2.881377140825705</v>
+        <v>4.117455860079382</v>
       </c>
       <c r="N36" t="n">
-        <v>0.3091152749195752</v>
+        <v>0.001677748274402553</v>
       </c>
       <c r="O36" t="n">
-        <v>0.896322936052222</v>
+        <v>1.038442633023389</v>
       </c>
       <c r="P36" t="n">
-        <v>0.7967247306056913</v>
+        <v>0.02060491692789433</v>
       </c>
       <c r="Q36" t="n">
-        <v>1.008371869017438</v>
+        <v>52.3352317242636</v>
       </c>
       <c r="R36" t="n">
-        <v>0.07093033261618928</v>
+        <v>1</v>
       </c>
       <c r="S36" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -2953,64 +2953,64 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>carriers_pop+bridges_pop</t>
+          <t>carriers_all+bridges_all</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>idr</t>
+          <t>ard</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F37" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G37" t="n">
-        <v>437</v>
+        <v>166</v>
       </c>
       <c r="H37" t="n">
-        <v>520</v>
+        <v>159</v>
       </c>
       <c r="I37" t="n">
-        <v>81073</v>
+        <v>100019</v>
       </c>
       <c r="J37" t="n">
-        <v>83247</v>
+        <v>89328</v>
       </c>
       <c r="K37" t="n">
-        <v>1.848267610671864</v>
+        <v>3.929685359781641</v>
       </c>
       <c r="L37" t="n">
-        <v>0.8531397260688854</v>
+        <v>1.488077837107677</v>
       </c>
       <c r="M37" t="n">
-        <v>4.004142646597195</v>
+        <v>10.37743231019223</v>
       </c>
       <c r="N37" t="n">
-        <v>0.1317787070408102</v>
+        <v>0.003124934066074294</v>
       </c>
       <c r="O37" t="n">
-        <v>0.8629198139568424</v>
+        <v>0.9324296308229738</v>
       </c>
       <c r="P37" t="n">
-        <v>0.7595772962299928</v>
+        <v>0.750033348347161</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.980322356941331</v>
+        <v>1.159181812852201</v>
       </c>
       <c r="R37" t="n">
-        <v>0.02522653355686949</v>
+        <v>0.5410616604028184</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -3022,60 +3022,60 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>carriers_all+bridges_all</t>
+          <t>carriers_pop+bridges_pop</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>miss</t>
+          <t>ard</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="F38" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="G38" t="n">
-        <v>1635</v>
+        <v>133</v>
       </c>
       <c r="H38" t="n">
-        <v>1517</v>
+        <v>147</v>
       </c>
       <c r="I38" t="n">
-        <v>100019</v>
+        <v>81073</v>
       </c>
       <c r="J38" t="n">
-        <v>89328</v>
+        <v>83247</v>
       </c>
       <c r="K38" t="n">
-        <v>1.822674100084249</v>
+        <v>3.491172153491298</v>
       </c>
       <c r="L38" t="n">
-        <v>1.294867473029087</v>
+        <v>1.287966744809779</v>
       </c>
       <c r="M38" t="n">
-        <v>2.565622308317344</v>
+        <v>9.463196976497366</v>
       </c>
       <c r="N38" t="n">
-        <v>0.0005235257631555407</v>
+        <v>0.009761027862927318</v>
       </c>
       <c r="O38" t="n">
-        <v>0.9625809856839131</v>
+        <v>0.929023402189561</v>
       </c>
       <c r="P38" t="n">
-        <v>0.8971007867811498</v>
+        <v>0.7346401305548933</v>
       </c>
       <c r="Q38" t="n">
-        <v>1.032840643607921</v>
+        <v>1.174839824178888</v>
       </c>
       <c r="R38" t="n">
-        <v>0.2886359386058524</v>
+        <v>0.5501824510822202</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
@@ -3091,64 +3091,64 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>carriers_pop+bridges_pop</t>
+          <t>carriers_all+bridges_all</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>miss</t>
+          <t>brct</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="F39" t="n">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="G39" t="n">
-        <v>1303</v>
+        <v>576</v>
       </c>
       <c r="H39" t="n">
-        <v>1413</v>
+        <v>486</v>
       </c>
       <c r="I39" t="n">
-        <v>81073</v>
+        <v>100019</v>
       </c>
       <c r="J39" t="n">
-        <v>83247</v>
+        <v>89328</v>
       </c>
       <c r="K39" t="n">
-        <v>1.718799589634463</v>
+        <v>1.587751660517835</v>
       </c>
       <c r="L39" t="n">
-        <v>1.192747861919551</v>
+        <v>0.9907813391008043</v>
       </c>
       <c r="M39" t="n">
-        <v>2.476862146349296</v>
+        <v>2.544411401374462</v>
       </c>
       <c r="N39" t="n">
-        <v>0.003741190235494418</v>
+        <v>0.0635612054843895</v>
       </c>
       <c r="O39" t="n">
-        <v>0.9468792548185258</v>
+        <v>1.05850110701189</v>
       </c>
       <c r="P39" t="n">
-        <v>0.8776734764007882</v>
+        <v>0.9378142779619217</v>
       </c>
       <c r="Q39" t="n">
-        <v>1.021542005441968</v>
+        <v>1.194719060985432</v>
       </c>
       <c r="R39" t="n">
-        <v>0.1635931973395008</v>
+        <v>0.3714346897558351</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -3160,60 +3160,60 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>carriers_all+bridges_all</t>
+          <t>carriers_pop+bridges_pop</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ring</t>
+          <t>brct</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F40" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G40" t="n">
-        <v>129</v>
+        <v>447</v>
       </c>
       <c r="H40" t="n">
-        <v>152</v>
+        <v>453</v>
       </c>
       <c r="I40" t="n">
-        <v>100019</v>
+        <v>81073</v>
       </c>
       <c r="J40" t="n">
-        <v>89328</v>
+        <v>83247</v>
       </c>
       <c r="K40" t="n">
-        <v>2.679330927123846</v>
+        <v>1.254996525764846</v>
       </c>
       <c r="L40" t="n">
-        <v>0.7253458527962984</v>
+        <v>0.7545987738475224</v>
       </c>
       <c r="M40" t="n">
-        <v>9.897091421102244</v>
+        <v>2.087223481229888</v>
       </c>
       <c r="N40" t="n">
-        <v>0.153684184993374</v>
+        <v>0.4388720879615608</v>
       </c>
       <c r="O40" t="n">
-        <v>0.7579686175416145</v>
+        <v>1.013215136093111</v>
       </c>
       <c r="P40" t="n">
-        <v>0.5993453556785866</v>
+        <v>0.8887884914462424</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.9585732495206727</v>
+        <v>1.155060986824529</v>
       </c>
       <c r="R40" t="n">
-        <v>0.02291922339128761</v>
+        <v>0.8672748777633897</v>
       </c>
       <c r="S40" t="inlineStr">
         <is>
@@ -3229,60 +3229,60 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>pop</t>
+          <t>all</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>carriers_pop+bridges_pop</t>
+          <t>carriers_all+bridges_all</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ring</t>
+          <t>idr</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F41" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G41" t="n">
-        <v>108</v>
+        <v>558</v>
       </c>
       <c r="H41" t="n">
-        <v>143</v>
+        <v>556</v>
       </c>
       <c r="I41" t="n">
-        <v>81073</v>
+        <v>100019</v>
       </c>
       <c r="J41" t="n">
-        <v>83247</v>
+        <v>89328</v>
       </c>
       <c r="K41" t="n">
-        <v>3.080446017786439</v>
+        <v>1.442716653066687</v>
       </c>
       <c r="L41" t="n">
-        <v>0.8339314720189192</v>
+        <v>0.7223737953440815</v>
       </c>
       <c r="M41" t="n">
-        <v>11.37880987453732</v>
+        <v>2.881377140825705</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0883310672484553</v>
+        <v>0.3091152749195752</v>
       </c>
       <c r="O41" t="n">
-        <v>0.7754968995826002</v>
+        <v>0.896322936052222</v>
       </c>
       <c r="P41" t="n">
-        <v>0.6039262639171159</v>
+        <v>0.7967247306056913</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.995809384678064</v>
+        <v>1.008371869017438</v>
       </c>
       <c r="R41" t="n">
-        <v>0.05003149692229729</v>
+        <v>0.07093033261618928</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
@@ -3298,64 +3298,64 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>pop</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>carriers_all+bridges_all</t>
+          <t>carriers_pop+bridges_pop</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>structured</t>
+          <t>idr</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F42" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="G42" t="n">
-        <v>871</v>
+        <v>437</v>
       </c>
       <c r="H42" t="n">
-        <v>797</v>
+        <v>520</v>
       </c>
       <c r="I42" t="n">
-        <v>100019</v>
+        <v>81073</v>
       </c>
       <c r="J42" t="n">
-        <v>89328</v>
+        <v>83247</v>
       </c>
       <c r="K42" t="n">
-        <v>2.01587755469318</v>
+        <v>1.848267610671864</v>
       </c>
       <c r="L42" t="n">
-        <v>1.353887314685857</v>
+        <v>0.8531397260688854</v>
       </c>
       <c r="M42" t="n">
-        <v>3.001551363570218</v>
+        <v>4.004142646597195</v>
       </c>
       <c r="N42" t="n">
-        <v>0.00046534560063148</v>
+        <v>0.1317787070408102</v>
       </c>
       <c r="O42" t="n">
-        <v>0.9760339763801213</v>
+        <v>0.8629198139568424</v>
       </c>
       <c r="P42" t="n">
-        <v>0.8862509911511173</v>
+        <v>0.7595772962299928</v>
       </c>
       <c r="Q42" t="n">
-        <v>1.07491256152057</v>
+        <v>0.980322356941331</v>
       </c>
       <c r="R42" t="n">
-        <v>0.6223760917437067</v>
+        <v>0.02522653355686949</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -3367,62 +3367,545 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>carriers_all+bridges_all</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>miss</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>100</v>
+      </c>
+      <c r="F43" t="n">
+        <v>49</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1635</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1517</v>
+      </c>
+      <c r="I43" t="n">
+        <v>100019</v>
+      </c>
+      <c r="J43" t="n">
+        <v>89328</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1.822674100084249</v>
+      </c>
+      <c r="L43" t="n">
+        <v>1.294867473029087</v>
+      </c>
+      <c r="M43" t="n">
+        <v>2.565622308317344</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.0005235257631555407</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.9625809856839131</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.8971007867811498</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>1.032840643607921</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.2886359386058524</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>pop</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>carriers_pop+bridges_pop</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>miss</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>77</v>
+      </c>
+      <c r="F44" t="n">
+        <v>46</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1303</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1413</v>
+      </c>
+      <c r="I44" t="n">
+        <v>81073</v>
+      </c>
+      <c r="J44" t="n">
+        <v>83247</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1.718799589634463</v>
+      </c>
+      <c r="L44" t="n">
+        <v>1.192747861919551</v>
+      </c>
+      <c r="M44" t="n">
+        <v>2.476862146349296</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0.003741190235494418</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.9468792548185258</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.8776734764007882</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>1.021542005441968</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0.1635931973395008</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>carriers_all+bridges_all</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>ptv</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>74</v>
+      </c>
+      <c r="F45" t="n">
+        <v>38</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>100019</v>
+      </c>
+      <c r="J45" t="n">
+        <v>89328</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1.739214812343549</v>
+      </c>
+      <c r="L45" t="n">
+        <v>1.176065094217926</v>
+      </c>
+      <c r="M45" t="n">
+        <v>2.572024438397882</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0.005809188042755499</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.4465551545206411</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.0149811647106033</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>13.31081460494291</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0.4717715529132894</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>carriers_pop+bridges_pop</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ptv</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>60</v>
+      </c>
+      <c r="F46" t="n">
+        <v>36</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>81073</v>
+      </c>
+      <c r="J46" t="n">
+        <v>83247</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1.711358898770244</v>
+      </c>
+      <c r="L46" t="n">
+        <v>1.131990835277625</v>
+      </c>
+      <c r="M46" t="n">
+        <v>2.587255293177185</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.01055371444153883</v>
+      </c>
+      <c r="O46" t="n">
+        <v>1.026815339262146</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.02037436491669925</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>51.74883954688908</v>
+      </c>
+      <c r="R46" t="n">
+        <v>1</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>carriers_all+bridges_all</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>ring</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>9</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3</v>
+      </c>
+      <c r="G47" t="n">
+        <v>129</v>
+      </c>
+      <c r="H47" t="n">
+        <v>152</v>
+      </c>
+      <c r="I47" t="n">
+        <v>100019</v>
+      </c>
+      <c r="J47" t="n">
+        <v>89328</v>
+      </c>
+      <c r="K47" t="n">
+        <v>2.679330927123846</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.7253458527962984</v>
+      </c>
+      <c r="M47" t="n">
+        <v>9.897091421102244</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.153684184993374</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.7579686175416145</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0.5993453556785866</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.9585732495206727</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0.02291922339128761</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>carriers_pop+bridges_pop</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>ring</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>9</v>
+      </c>
+      <c r="F48" t="n">
+        <v>3</v>
+      </c>
+      <c r="G48" t="n">
+        <v>108</v>
+      </c>
+      <c r="H48" t="n">
+        <v>143</v>
+      </c>
+      <c r="I48" t="n">
+        <v>81073</v>
+      </c>
+      <c r="J48" t="n">
+        <v>83247</v>
+      </c>
+      <c r="K48" t="n">
+        <v>3.080446017786439</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.8339314720189192</v>
+      </c>
+      <c r="M48" t="n">
+        <v>11.37880987453732</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.0883310672484553</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.7754968995826002</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0.6039262639171159</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.995809384678064</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0.05003149692229729</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>carriers_all+bridges_all</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
         <is>
           <t>structured</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="E49" t="n">
+        <v>79</v>
+      </c>
+      <c r="F49" t="n">
+        <v>35</v>
+      </c>
+      <c r="G49" t="n">
+        <v>871</v>
+      </c>
+      <c r="H49" t="n">
+        <v>797</v>
+      </c>
+      <c r="I49" t="n">
+        <v>100019</v>
+      </c>
+      <c r="J49" t="n">
+        <v>89328</v>
+      </c>
+      <c r="K49" t="n">
+        <v>2.01587755469318</v>
+      </c>
+      <c r="L49" t="n">
+        <v>1.353887314685857</v>
+      </c>
+      <c r="M49" t="n">
+        <v>3.001551363570218</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.00046534560063148</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.9760339763801213</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.8862509911511173</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>1.07491256152057</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0.6223760917437067</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>carriers+bridges</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>carriers_pop+bridges_pop</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>structured</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
         <v>59</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F50" t="n">
         <v>35</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G50" t="n">
         <v>688</v>
       </c>
-      <c r="H43" t="n">
+      <c r="H50" t="n">
         <v>743</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I50" t="n">
         <v>81073</v>
       </c>
-      <c r="J43" t="n">
+      <c r="J50" t="n">
         <v>83247</v>
       </c>
-      <c r="K43" t="n">
+      <c r="K50" t="n">
         <v>1.730917286184761</v>
       </c>
-      <c r="L43" t="n">
+      <c r="L50" t="n">
         <v>1.139250427027606</v>
       </c>
-      <c r="M43" t="n">
+      <c r="M50" t="n">
         <v>2.629864848442682</v>
       </c>
-      <c r="N43" t="n">
+      <c r="N50" t="n">
         <v>0.0097652207222705</v>
       </c>
-      <c r="O43" t="n">
+      <c r="O50" t="n">
         <v>0.9508061284150159</v>
       </c>
-      <c r="P43" t="n">
+      <c r="P50" t="n">
         <v>0.8567619232849841</v>
       </c>
-      <c r="Q43" t="n">
+      <c r="Q50" t="n">
         <v>1.055173285905754</v>
       </c>
-      <c r="R43" t="n">
+      <c r="R50" t="n">
         <v>0.3527322904673619</v>
       </c>
-      <c r="S43" t="inlineStr">
+      <c r="S50" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>

</xml_diff>